<commit_message>
Uploaded the new sample excel file with advanced lookup fields for options.
</commit_message>
<xml_diff>
--- a/static/sample_orders.xlsx
+++ b/static/sample_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,21 @@
           <t>Tag</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>StrikePrice</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ExpiryDate</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>OptionType</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -533,28 +548,31 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Sample Order 1</t>
-        </is>
-      </c>
+          <t>Stock Order</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RELIANCE</t>
+          <t>BSXOPT</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>BFO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SELL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -562,7 +580,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2500</v>
+        <v>138</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -570,29 +588,42 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>2400</v>
+        <v>238</v>
       </c>
       <c r="I3" t="n">
-        <v>2600</v>
+        <v>90</v>
       </c>
       <c r="J3" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sample Order 2</t>
+          <t>SENSEX PUT 85000</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>85000</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>2025-12-18</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>PE</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TCS</t>
+          <t>BSXOPT</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>BFO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -601,43 +632,58 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>MARKET</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>140</v>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>CNC</t>
+          <t>INTRADAY</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>3800</v>
+        <v>240</v>
       </c>
       <c r="I4" t="n">
-        <v>3500</v>
+        <v>92</v>
       </c>
       <c r="J4" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Market Order Example</t>
+          <t>SENSEX PUT 84900</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>84900</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>2025-12-18</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>PE</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>INFY</t>
+          <t>NIFTY-Dec2025-24000-CE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>NSE_FNO</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -646,7 +692,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -654,7 +700,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1450</v>
+        <v>100</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -662,19 +708,22 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="I5" t="n">
-        <v>1420</v>
+        <v>80</v>
       </c>
       <c r="J5" t="n">
         <v>5</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Intraday Order</t>
-        </is>
-      </c>
+          <t>NIFTY Call</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added support for forever orders
</commit_message>
<xml_diff>
--- a/static/sample_orders.xlsx
+++ b/static/sample_orders.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Orders" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,70 +436,110 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>DhanOrderType</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Symbol</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Exchange</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>TransactionType</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>OrderType</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ProductType</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ProductType</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>TargetPrice</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>StopLoss</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>TrailingStopLoss</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>TriggerPrice</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OrderFlag</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Validity</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>DisclosedQuantity</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Price1</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>TriggerPrice1</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity1</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Tag</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>StrikePrice</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>ExpiryDate</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>OptionType</t>
         </is>
@@ -508,222 +548,348 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HDFCBANK</t>
+          <t>SUPER</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>SBIN</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>BUY</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>LIMIT</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>1500</v>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>CNC</t>
+          <t>INTRADAY</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1600</v>
+        <v>610</v>
       </c>
       <c r="I2" t="n">
-        <v>1400</v>
+        <v>650</v>
       </c>
       <c r="J2" t="n">
-        <v>10</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Stock Order</t>
-        </is>
+        <v>590</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BSXOPT</t>
+          <t>FOREVER</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BFO</t>
+          <t>SBIN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>BUY</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>60</v>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>LIMIT</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>138</v>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>INTRADAY</t>
+          <t>CNC</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>238</v>
-      </c>
-      <c r="I3" t="n">
-        <v>90</v>
-      </c>
-      <c r="J3" t="n">
-        <v>5</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>SENSEX PUT 85000</t>
-        </is>
-      </c>
+        <v>1428</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
-        <v>85000</v>
+        <v>1427</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>SINGLE</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>PE</t>
-        </is>
-      </c>
+          <t>DAY</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>1</v>
+      </c>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>my_strategy</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BSXOPT</t>
+          <t>FOREVER</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BFO</t>
+          <t>RELIANCE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>BUY</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>60</v>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>LIMIT</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>140</v>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>INTRADAY</t>
+          <t>CNC</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>240</v>
-      </c>
-      <c r="I4" t="n">
-        <v>92</v>
-      </c>
-      <c r="J4" t="n">
-        <v>5</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>SENSEX PUT 84900</t>
-        </is>
-      </c>
+        <v>2428</v>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="n">
-        <v>84900</v>
+        <v>2427</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>OCO</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>PE</t>
-        </is>
-      </c>
+          <t>DAY</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2420</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2419</v>
+      </c>
+      <c r="R4" t="n">
+        <v>10</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>my_strategy_oco</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NIFTY-Dec2025-24000-CE</t>
+          <t>SUPER</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NSE_FNO</t>
+          <t>NIFTY</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>BUY</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>50</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>LIMIT</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>100</v>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
           <t>INTRADAY</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>150</v>
+        <v>100.5</v>
       </c>
       <c r="I5" t="n">
+        <v>120</v>
+      </c>
+      <c r="J5" t="n">
         <v>80</v>
       </c>
-      <c r="J5" t="n">
-        <v>5</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>NIFTY Call</t>
-        </is>
+      <c r="K5" t="n">
+        <v>0</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="n">
+        <v>24000</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>2025-12-18</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FOREVER</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BSXOPT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BFO</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>LIMIT</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>CNC</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>250</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>245</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>SINGLE</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>DAY</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>sensex_forever</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>2025-12-18</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>